<commit_message>
raster plots for bursts
</commit_message>
<xml_diff>
--- a/muna-disentanglement/meaTable.xlsx
+++ b/muna-disentanglement/meaTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="full" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="147">
   <si>
     <t>genotype</t>
   </si>
@@ -33,9 +33,6 @@
     <t>maxRecording</t>
   </si>
   <si>
-    <t>excludeChannels</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -387,73 +384,88 @@
     <t>31,41,71,42,43,83</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">75,84, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>no: 31,62,33,53,34,74,58</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>34,33,62,82,75,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> no: 31,41,22,72,53,54,74,25,16,26,36,17,27,37,47,58,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>55,56,57,58,68,47</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> no: 31,62,33,13,53,74,34</t>
-    </r>
-  </si>
-  <si>
-    <t>31,41,61,71,32,42,52,33,43,53,54,83,25</t>
+    <t>channels2exclude</t>
+  </si>
+  <si>
+    <t>55,56,57,58,68,47</t>
+  </si>
+  <si>
+    <t>no: 31,62,33,13,53,74,34</t>
+  </si>
+  <si>
+    <t>34,33,62,82,75</t>
+  </si>
+  <si>
+    <t>no: 31,41,22,72,53,54,74,25,16,26,36,17,27,37,47,58</t>
+  </si>
+  <si>
+    <t>75,84</t>
+  </si>
+  <si>
+    <t>no: 31,62,33,53,34,74,58</t>
+  </si>
+  <si>
+    <t>31,41,12,32,42,52,43,33,72,83,15,25</t>
+  </si>
+  <si>
+    <t>noisy, signals missed</t>
+  </si>
+  <si>
+    <t>no: 62,13,33,53,82,34,74</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>no: 34,82,58</t>
+  </si>
+  <si>
+    <t>82,34,75,58,78</t>
+  </si>
+  <si>
+    <t>no: 51,62,24,45,37,57</t>
+  </si>
+  <si>
+    <t>16,23,33,54,61,71,83,31</t>
+  </si>
+  <si>
+    <t>31,61,71,12,42,62,83,23,33</t>
+  </si>
+  <si>
+    <t>41,71,32,42,83,23,33,43,25,35,45</t>
+  </si>
+  <si>
+    <t>31,41,61,71,42,52,43,53,83,15,25,16</t>
+  </si>
+  <si>
+    <t>13,66</t>
+  </si>
+  <si>
+    <t>small signals not detected</t>
+  </si>
+  <si>
+    <t>no:31,62,82,13,33,53,34,74,58</t>
+  </si>
+  <si>
+    <t>no:31,62,82,13,33,53,34,74,59</t>
+  </si>
+  <si>
+    <t>nice; last 2 mins discarded due to noise</t>
+  </si>
+  <si>
+    <t>nice; last 10 mins discarded due to noise</t>
+  </si>
+  <si>
+    <t>55, 56,57,58,68,47</t>
+  </si>
+  <si>
+    <t>no 31,41,22,72,53,54,74,25,16,26,36,17,27,37,47,58</t>
+  </si>
+  <si>
+    <t>no: 82,34,84,58</t>
+  </si>
+  <si>
+    <t>variable noise</t>
   </si>
 </sst>
 </file>
@@ -502,13 +514,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -792,7 +805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -808,19 +821,19 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -829,13 +842,16 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>129</v>
       </c>
       <c r="Q1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -843,28 +859,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -872,28 +891,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -901,25 +923,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
         <v>66</v>
       </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -927,19 +952,28 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
         <v>68</v>
       </c>
-      <c r="E5" t="s">
-        <v>69</v>
-      </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>52</v>
+      </c>
+      <c r="H5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -947,19 +981,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
         <v>70</v>
       </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>60</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -967,19 +1010,25 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
         <v>72</v>
       </c>
-      <c r="E7" t="s">
-        <v>73</v>
-      </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>60</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -987,19 +1036,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" t="s">
         <v>74</v>
       </c>
-      <c r="E8" t="s">
-        <v>75</v>
-      </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1007,19 +1059,28 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" t="s">
         <v>76</v>
       </c>
-      <c r="E9" t="s">
-        <v>77</v>
-      </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>60</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1027,19 +1088,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
         <v>78</v>
       </c>
-      <c r="E10" t="s">
-        <v>79</v>
-      </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1047,19 +1108,28 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
       <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
         <v>80</v>
       </c>
-      <c r="E11" t="s">
-        <v>81</v>
-      </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>60</v>
+      </c>
+      <c r="H11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1067,19 +1137,28 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
       <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
         <v>82</v>
       </c>
-      <c r="E12" t="s">
-        <v>83</v>
-      </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1087,19 +1166,28 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
       <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
         <v>84</v>
       </c>
-      <c r="E13" t="s">
-        <v>85</v>
-      </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="G13">
+        <v>53</v>
+      </c>
+      <c r="H13" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1107,19 +1195,28 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
       <c r="D14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" t="s">
         <v>86</v>
       </c>
-      <c r="E14" t="s">
-        <v>87</v>
-      </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
+        <v>136</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1127,25 +1224,28 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
       <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" t="s">
         <v>88</v>
       </c>
-      <c r="E15" t="s">
-        <v>89</v>
-      </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>46</v>
       </c>
       <c r="H15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1153,28 +1253,28 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
       <c r="D16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" t="s">
         <v>90</v>
       </c>
-      <c r="E16" t="s">
-        <v>91</v>
-      </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1182,205 +1282,298 @@
         <v>180122</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" t="s">
         <v>92</v>
       </c>
-      <c r="E17" t="s">
-        <v>93</v>
-      </c>
       <c r="F17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
       <c r="D18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" t="s">
         <v>94</v>
       </c>
-      <c r="E18" t="s">
-        <v>95</v>
-      </c>
       <c r="F18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G18">
+        <v>60</v>
+      </c>
+      <c r="I18" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
       <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
       <c r="D19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" t="s">
         <v>96</v>
       </c>
-      <c r="E19" t="s">
-        <v>97</v>
-      </c>
       <c r="F19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G19">
+        <v>62</v>
+      </c>
+      <c r="I19" t="s">
+        <v>114</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
       <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
       <c r="D20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" t="s">
         <v>98</v>
       </c>
-      <c r="E20" t="s">
-        <v>99</v>
-      </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="G20">
+        <v>20</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="I20" t="s">
+        <v>141</v>
+      </c>
+      <c r="J20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
       <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
         <v>51</v>
       </c>
-      <c r="C21" t="s">
-        <v>52</v>
-      </c>
       <c r="D21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" t="s">
         <v>100</v>
       </c>
-      <c r="E21" t="s">
-        <v>101</v>
-      </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="I21" t="s">
+        <v>142</v>
+      </c>
+      <c r="J21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
       <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
         <v>53</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>27</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" t="s">
+        <v>114</v>
+      </c>
+      <c r="J22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
         <v>54</v>
       </c>
-      <c r="D22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
         <v>103</v>
       </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23">
+        <v>60</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="D23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
         <v>105</v>
       </c>
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>106</v>
       </c>
-      <c r="E24" t="s">
-        <v>107</v>
-      </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="G24">
+        <v>50</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" t="s">
         <v>108</v>
       </c>
-      <c r="E25" t="s">
-        <v>109</v>
-      </c>
       <c r="F25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <v>60</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>15</v>
       </c>
       <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
         <v>60</v>
       </c>
-      <c r="C26" t="s">
-        <v>61</v>
-      </c>
       <c r="D26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
         <v>110</v>
       </c>
-      <c r="E26" t="s">
-        <v>111</v>
-      </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="G26">
+        <v>60</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1390,10 +1583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,19 +1603,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -1431,10 +1624,10 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1442,144 +1635,57 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>118</v>
-      </c>
-      <c r="I4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>46</v>
-      </c>
-      <c r="H5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6">
-        <v>47</v>
-      </c>
-      <c r="H6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>